<commit_message>
updates of online TC
updates of online TC
</commit_message>
<xml_diff>
--- a/_assets_/tc.xlsx
+++ b/_assets_/tc.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>SCHOOL_NO</t>
   </si>
@@ -92,6 +92,24 @@
   </si>
   <si>
     <t>REMARKS_IF_ANY</t>
+  </si>
+  <si>
+    <t>RENEWED_UPTO</t>
+  </si>
+  <si>
+    <t>SCHOOL_STATUS</t>
+  </si>
+  <si>
+    <t>CLASS</t>
+  </si>
+  <si>
+    <t>CANDIDATE_ADHAAR</t>
+  </si>
+  <si>
+    <t>MOTHER_ADHAAR</t>
+  </si>
+  <si>
+    <t>FATHER_ADHAAR</t>
   </si>
 </sst>
 </file>
@@ -576,8 +594,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -913,123 +932,146 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Z1"/>
+  <dimension ref="A1:AF1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0">
-      <selection activeCell="Z1" sqref="Z1:Z1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="26.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="24.5703125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="29.140625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="27.28515625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="31.85546875" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="16" customWidth="1"/>
+    <col min="9" max="9" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18" customWidth="1"/>
+    <col min="12" max="12" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.28515625" customWidth="1"/>
+    <col min="14" max="14" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.85546875" customWidth="1"/>
+    <col min="16" max="16" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="24.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="29.140625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="31.85546875" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="16.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26">
+    <row r="1" spans="1:32">
       <c r="A1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="J1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="K1" t="s">
+        <v>29</v>
+      </c>
+      <c r="L1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="M1" t="s">
+        <v>30</v>
+      </c>
+      <c r="N1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="O1" t="s">
+        <v>31</v>
+      </c>
+      <c r="P1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="R1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="S1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="T1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="U1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="V1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="W1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" t="s">
+      <c r="X1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" t="s">
+      <c r="Y1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" t="s">
+      <c r="Z1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" t="s">
+      <c r="AB1" t="s">
         <v>21</v>
       </c>
-      <c r="W1" t="s">
+      <c r="AC1" t="s">
         <v>22</v>
       </c>
-      <c r="X1" t="s">
+      <c r="AD1" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="AE1" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AF1" t="s">
         <v>25</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>